<commit_message>
corrected filter in wthr_generation_fns.py
</commit_message>
<xml_diff>
--- a/docs/World_divisions.xlsx
+++ b/docs/World_divisions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AbUniv\GlblEcosseSiteSpecSv\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AbUnivGit\SoilsRGreatGlEc\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87B09E7-4DEC-4E20-9180-1DE3DD43E380}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677C2A78-F1CB-4628-8420-22A927AB701A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31320" yWindow="405" windowWidth="24390" windowHeight="14565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32250" yWindow="600" windowWidth="23985" windowHeight="16275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="1" r:id="rId1"/>
@@ -446,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -494,23 +494,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -586,9 +582,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -626,7 +622,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -732,7 +728,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -874,7 +870,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -885,7 +881,7 @@
   <dimension ref="A1:AA17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -975,126 +971,123 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="28" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A2" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="28">
-        <v>-166</v>
-      </c>
-      <c r="C2" s="28">
-        <v>-33</v>
-      </c>
-      <c r="D2" s="28">
-        <v>12</v>
-      </c>
-      <c r="E2" s="28">
-        <v>75</v>
-      </c>
-      <c r="F2" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="30">
+    <row r="2" spans="1:27" s="26" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2">
+        <v>-20</v>
+      </c>
+      <c r="C2" s="2">
+        <v>56</v>
+      </c>
+      <c r="D2" s="2">
+        <v>-41.5</v>
+      </c>
+      <c r="E2" s="2">
+        <v>17</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="8">
         <f>I2*3600</f>
-        <v>18032400</v>
-      </c>
-      <c r="I2" s="31">
-        <v>5009</v>
-      </c>
-      <c r="J2" s="31">
-        <v>26230</v>
-      </c>
-      <c r="K2" s="31">
+        <v>17506800</v>
+      </c>
+      <c r="I2" s="10">
+        <v>4863</v>
+      </c>
+      <c r="J2" s="3">
+        <v>13344</v>
+      </c>
+      <c r="K2" s="3">
         <f>I2+J2</f>
-        <v>31239</v>
-      </c>
-      <c r="L2" s="32">
+        <v>18207</v>
+      </c>
+      <c r="L2" s="4">
         <f>I2/K2</f>
-        <v>0.16034444124331765</v>
-      </c>
-      <c r="N2" s="31">
+        <v>0.26709507332344701</v>
+      </c>
+      <c r="N2" s="29">
         <v>17820</v>
       </c>
-      <c r="O2" s="31">
+      <c r="O2" s="29">
         <v>106369</v>
       </c>
-      <c r="P2" s="31">
+      <c r="P2" s="29">
         <f>N2+O2</f>
         <v>124189</v>
       </c>
-      <c r="Q2" s="32">
+      <c r="Q2" s="30">
         <f>N2/P2</f>
         <v>0.14349096940952902</v>
       </c>
-      <c r="S2" s="31">
-        <v>0</v>
-      </c>
-      <c r="T2" s="31">
+      <c r="S2" s="29">
+        <v>0</v>
+      </c>
+      <c r="T2" s="29">
         <v>26230</v>
       </c>
-      <c r="U2" s="31">
+      <c r="U2" s="29">
         <f>S2+T2</f>
         <v>26230</v>
       </c>
-      <c r="V2" s="32">
+      <c r="V2" s="30">
         <f>S2/U2</f>
         <v>0</v>
       </c>
-      <c r="X2" s="31">
+      <c r="X2" s="29">
         <v>2593</v>
       </c>
-      <c r="Y2" s="31">
+      <c r="Y2" s="29">
         <v>121596</v>
       </c>
-      <c r="Z2" s="31">
+      <c r="Z2" s="29">
         <f>X2+Y2</f>
         <v>124189</v>
       </c>
-      <c r="AA2" s="32">
+      <c r="AA2" s="30">
         <f>X2/Z2</f>
         <v>2.0879465975247403E-2</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="20.100000000000001" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2">
-        <f>B2</f>
-        <v>-166</v>
+        <v>50</v>
       </c>
       <c r="C3" s="2">
-        <v>-33</v>
+        <v>145</v>
       </c>
       <c r="D3" s="2">
-        <v>-60</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2">
-        <v>12</v>
-      </c>
-      <c r="F3" s="34" t="s">
-        <v>79</v>
+        <v>75</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>81</v>
       </c>
       <c r="H3" s="8">
-        <f t="shared" ref="H3:H7" si="0">I3*3600</f>
-        <v>10994400</v>
+        <f>I3*3600</f>
+        <v>34621200</v>
       </c>
       <c r="I3" s="10">
-        <v>3054</v>
+        <v>9617</v>
       </c>
       <c r="J3" s="3">
-        <v>35661</v>
+        <v>14640</v>
       </c>
       <c r="K3" s="3">
-        <f t="shared" ref="K3:K7" si="1">I3+J3</f>
-        <v>38715</v>
+        <f>I3+J3</f>
+        <v>24257</v>
       </c>
       <c r="L3" s="4">
-        <f t="shared" ref="L3:L7" si="2">I3/K3</f>
-        <v>7.8884153428903522E-2</v>
+        <f>I3/K3</f>
+        <v>0.39646287669538688</v>
       </c>
       <c r="N3" s="10">
         <v>10837</v>
@@ -1103,11 +1096,11 @@
         <v>143200</v>
       </c>
       <c r="P3" s="3">
-        <f t="shared" ref="P3:P7" si="3">N3+O3</f>
+        <f t="shared" ref="P3:P7" si="0">N3+O3</f>
         <v>154037</v>
       </c>
       <c r="Q3" s="4">
-        <f t="shared" ref="Q3:Q7" si="4">N3/P3</f>
+        <f t="shared" ref="Q3:Q7" si="1">N3/P3</f>
         <v>7.0353226822127149E-2</v>
       </c>
       <c r="S3" s="3">
@@ -1117,11 +1110,11 @@
         <v>35661</v>
       </c>
       <c r="U3" s="3">
-        <f t="shared" ref="U3:U7" si="5">S3+T3</f>
+        <f t="shared" ref="U3:U7" si="2">S3+T3</f>
         <v>35661</v>
       </c>
       <c r="V3" s="4">
-        <f t="shared" ref="V3:V7" si="6">S3/U3</f>
+        <f t="shared" ref="V3:V7" si="3">S3/U3</f>
         <v>0</v>
       </c>
       <c r="X3" s="3">
@@ -1131,131 +1124,132 @@
         <v>143200</v>
       </c>
       <c r="Z3" s="3">
-        <f t="shared" ref="Z3:Z7" si="7">X3+Y3</f>
+        <f t="shared" ref="Z3:Z7" si="4">X3+Y3</f>
         <v>143200</v>
       </c>
       <c r="AA3" s="4">
-        <f t="shared" ref="AA3:AA7" si="8">X3/Z3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" s="28" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="28" t="s">
+        <f t="shared" ref="AA3:AA7" si="5">X3/Z3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" s="26" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A4" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="26">
+        <v>112.5</v>
+      </c>
+      <c r="C4" s="26">
+        <v>179.1</v>
+      </c>
+      <c r="D4" s="26">
+        <v>-55.12</v>
+      </c>
+      <c r="E4" s="26">
+        <v>-9.2200000000000006</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" s="27"/>
+      <c r="H4" s="28">
+        <f>I4*3600</f>
+        <v>4410000</v>
+      </c>
+      <c r="I4" s="29">
+        <v>1225</v>
+      </c>
+      <c r="J4" s="29">
+        <v>11330</v>
+      </c>
+      <c r="K4" s="29">
+        <f>I4+J4</f>
+        <v>12555</v>
+      </c>
+      <c r="L4" s="30">
+        <f>I4/K4</f>
+        <v>9.7570688968538433E-2</v>
+      </c>
+      <c r="N4" s="29">
+        <v>19068</v>
+      </c>
+      <c r="O4" s="29">
+        <v>20699</v>
+      </c>
+      <c r="P4" s="29">
+        <f t="shared" si="0"/>
+        <v>39767</v>
+      </c>
+      <c r="Q4" s="30">
+        <f t="shared" si="1"/>
+        <v>0.47949304699876782</v>
+      </c>
+      <c r="S4" s="29">
+        <v>0</v>
+      </c>
+      <c r="T4" s="29">
+        <v>4788</v>
+      </c>
+      <c r="U4" s="29">
+        <f t="shared" si="2"/>
+        <v>4788</v>
+      </c>
+      <c r="V4" s="30">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="X4" s="29">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="29">
+        <v>20699</v>
+      </c>
+      <c r="Z4" s="29">
+        <f t="shared" si="4"/>
+        <v>20699</v>
+      </c>
+      <c r="AA4" s="30">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="20.100000000000001" customHeight="1">
+      <c r="A5" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B5" s="26">
         <v>-11.3</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C5" s="26">
         <v>50</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D5" s="26">
         <v>30</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E5" s="26">
         <v>75</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F5" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="G4" s="29"/>
-      <c r="H4" s="30">
-        <f t="shared" si="0"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="28">
+        <f>I5*3600</f>
         <v>18921600</v>
       </c>
-      <c r="I4" s="31">
+      <c r="I5" s="29">
         <v>5256</v>
       </c>
-      <c r="J4" s="31">
+      <c r="J5" s="29">
         <v>4788</v>
       </c>
-      <c r="K4" s="31">
-        <f t="shared" si="1"/>
+      <c r="K5" s="29">
+        <f>I5+J5</f>
         <v>10044</v>
       </c>
-      <c r="L4" s="32">
-        <f t="shared" si="2"/>
+      <c r="L5" s="30">
+        <f>I5/K5</f>
         <v>0.52329749103942658</v>
-      </c>
-      <c r="N4" s="31">
-        <v>19068</v>
-      </c>
-      <c r="O4" s="31">
-        <v>20699</v>
-      </c>
-      <c r="P4" s="31">
-        <f t="shared" si="3"/>
-        <v>39767</v>
-      </c>
-      <c r="Q4" s="32">
-        <f t="shared" si="4"/>
-        <v>0.47949304699876782</v>
-      </c>
-      <c r="S4" s="31">
-        <v>0</v>
-      </c>
-      <c r="T4" s="31">
-        <v>4788</v>
-      </c>
-      <c r="U4" s="31">
-        <f t="shared" si="5"/>
-        <v>4788</v>
-      </c>
-      <c r="V4" s="32">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X4" s="31">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="31">
-        <v>20699</v>
-      </c>
-      <c r="Z4" s="31">
-        <f t="shared" si="7"/>
-        <v>20699</v>
-      </c>
-      <c r="AA4" s="32">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2">
-        <v>50</v>
-      </c>
-      <c r="C5" s="2">
-        <v>145</v>
-      </c>
-      <c r="D5" s="2">
-        <v>7</v>
-      </c>
-      <c r="E5" s="2">
-        <v>75</v>
-      </c>
-      <c r="F5" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="H5" s="8">
-        <f t="shared" si="0"/>
-        <v>34621200</v>
-      </c>
-      <c r="I5" s="10">
-        <v>9617</v>
-      </c>
-      <c r="J5" s="3">
-        <v>14640</v>
-      </c>
-      <c r="K5" s="3">
-        <f t="shared" si="1"/>
-        <v>24257</v>
-      </c>
-      <c r="L5" s="4">
-        <f t="shared" si="2"/>
-        <v>0.39646287669538688</v>
       </c>
       <c r="N5" s="10">
         <v>34512</v>
@@ -1264,11 +1258,11 @@
         <v>61881</v>
       </c>
       <c r="P5" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>96393</v>
       </c>
       <c r="Q5" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>0.35803429709626217</v>
       </c>
       <c r="S5" s="3">
@@ -1278,11 +1272,11 @@
         <v>14640</v>
       </c>
       <c r="U5" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>14640</v>
       </c>
       <c r="V5" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="X5" s="3">
@@ -1292,131 +1286,134 @@
         <v>61881</v>
       </c>
       <c r="Z5" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>61881</v>
       </c>
       <c r="AA5" s="4">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" s="28" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="28">
-        <v>112.5</v>
-      </c>
-      <c r="C6" s="28">
-        <v>179.1</v>
-      </c>
-      <c r="D6" s="28">
-        <v>-55.12</v>
-      </c>
-      <c r="E6" s="28">
-        <v>-9.2200000000000006</v>
-      </c>
-      <c r="F6" s="33" t="s">
-        <v>82</v>
-      </c>
-      <c r="G6" s="29"/>
-      <c r="H6" s="30">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" s="26" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A6" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="26">
+        <v>-166</v>
+      </c>
+      <c r="C6" s="26">
+        <v>-33</v>
+      </c>
+      <c r="D6" s="26">
+        <v>12</v>
+      </c>
+      <c r="E6" s="26">
+        <v>75</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="28">
+        <f>I6*3600</f>
+        <v>18032400</v>
+      </c>
+      <c r="I6" s="29">
+        <v>5009</v>
+      </c>
+      <c r="J6" s="29">
+        <v>26230</v>
+      </c>
+      <c r="K6" s="29">
+        <f>I6+J6</f>
+        <v>31239</v>
+      </c>
+      <c r="L6" s="30">
+        <f>I6/K6</f>
+        <v>0.16034444124331765</v>
+      </c>
+      <c r="N6" s="29">
+        <v>3866</v>
+      </c>
+      <c r="O6" s="29">
+        <v>45529</v>
+      </c>
+      <c r="P6" s="29">
         <f t="shared" si="0"/>
-        <v>4410000</v>
-      </c>
-      <c r="I6" s="31">
-        <v>1225</v>
-      </c>
-      <c r="J6" s="31">
+        <v>49395</v>
+      </c>
+      <c r="Q6" s="30">
+        <f t="shared" si="1"/>
+        <v>7.8267031076019844E-2</v>
+      </c>
+      <c r="S6" s="29">
+        <v>0</v>
+      </c>
+      <c r="T6" s="29">
         <v>11330</v>
       </c>
-      <c r="K6" s="31">
-        <f t="shared" si="1"/>
-        <v>12555</v>
-      </c>
-      <c r="L6" s="32">
+      <c r="U6" s="29">
         <f t="shared" si="2"/>
-        <v>9.7570688968538433E-2</v>
-      </c>
-      <c r="N6" s="31">
-        <v>3866</v>
-      </c>
-      <c r="O6" s="31">
+        <v>11330</v>
+      </c>
+      <c r="V6" s="30">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="X6" s="29">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="29">
         <v>45529</v>
       </c>
-      <c r="P6" s="31">
-        <f t="shared" si="3"/>
-        <v>49395</v>
-      </c>
-      <c r="Q6" s="32">
+      <c r="Z6" s="29">
         <f t="shared" si="4"/>
-        <v>7.8267031076019844E-2</v>
-      </c>
-      <c r="S6" s="31">
-        <v>0</v>
-      </c>
-      <c r="T6" s="31">
-        <v>11330</v>
-      </c>
-      <c r="U6" s="31">
+        <v>45529</v>
+      </c>
+      <c r="AA6" s="30">
         <f t="shared" si="5"/>
-        <v>11330</v>
-      </c>
-      <c r="V6" s="32">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X6" s="31">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="31">
-        <v>45529</v>
-      </c>
-      <c r="Z6" s="31">
-        <f t="shared" si="7"/>
-        <v>45529</v>
-      </c>
-      <c r="AA6" s="32">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>-20</v>
+        <f>B6</f>
+        <v>-166</v>
       </c>
       <c r="C7" s="2">
-        <v>56</v>
+        <v>-33</v>
       </c>
       <c r="D7" s="2">
-        <v>-41.5</v>
+        <v>-60</v>
       </c>
       <c r="E7" s="2">
-        <v>17</v>
-      </c>
-      <c r="F7" s="34" t="s">
-        <v>83</v>
+        <v>12</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>79</v>
       </c>
       <c r="H7" s="8">
-        <f t="shared" si="0"/>
-        <v>17506800</v>
+        <f>I7*3600</f>
+        <v>10994400</v>
       </c>
       <c r="I7" s="10">
-        <v>4863</v>
+        <v>3054</v>
       </c>
       <c r="J7" s="3">
-        <v>13344</v>
+        <v>35661</v>
       </c>
       <c r="K7" s="3">
-        <f t="shared" si="1"/>
-        <v>18207</v>
+        <f>I7+J7</f>
+        <v>38715</v>
       </c>
       <c r="L7" s="4">
-        <f t="shared" si="2"/>
-        <v>0.26709507332344701</v>
+        <f>I7/K7</f>
+        <v>7.8884153428903522E-2</v>
       </c>
       <c r="N7" s="10">
         <v>17377</v>
@@ -1425,11 +1422,11 @@
         <v>54298</v>
       </c>
       <c r="P7" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>71675</v>
       </c>
       <c r="Q7" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>0.24244157656086501</v>
       </c>
       <c r="S7" s="3">
@@ -1439,11 +1436,11 @@
         <v>13344</v>
       </c>
       <c r="U7" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>13344</v>
       </c>
       <c r="V7" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="X7" s="3">
@@ -1453,69 +1450,72 @@
         <v>53973</v>
       </c>
       <c r="Z7" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>71675</v>
       </c>
       <c r="AA7" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>0.2469759330310429</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="20.100000000000001" customHeight="1">
-      <c r="F8" s="34"/>
+      <c r="F8" s="32"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:27" ht="20.100000000000001" customHeight="1">
-      <c r="F9" s="34"/>
+      <c r="F9" s="32"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:27" ht="20.100000000000001" customHeight="1">
-      <c r="F10" s="34"/>
+      <c r="F10" s="32"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:27" ht="20.100000000000001" customHeight="1">
-      <c r="F11" s="34"/>
+      <c r="F11" s="32"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
     </row>
     <row r="12" spans="1:27" ht="20.100000000000001" customHeight="1">
-      <c r="F12" s="34"/>
+      <c r="F12" s="32"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:27" ht="20.100000000000001" customHeight="1">
-      <c r="F13" s="34"/>
+      <c r="F13" s="32"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
     </row>
     <row r="14" spans="1:27" ht="20.100000000000001" customHeight="1">
-      <c r="F14" s="34"/>
+      <c r="F14" s="32"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:27" ht="20.100000000000001" customHeight="1">
-      <c r="F15" s="34"/>
+      <c r="F15" s="32"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
     <row r="16" spans="1:27" ht="20.100000000000001" customHeight="1">
-      <c r="F16" s="34"/>
+      <c r="F16" s="32"/>
     </row>
     <row r="17" spans="6:6" ht="20.100000000000001" customHeight="1">
-      <c r="F17" s="34"/>
+      <c r="F17" s="32"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L17">
+    <sortCondition ref="F1:F17"/>
+  </sortState>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -1848,294 +1848,294 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="18" customHeight="1">
-      <c r="B11" s="18">
+      <c r="B11" s="17">
         <v>16</v>
       </c>
-      <c r="C11" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="23" t="s">
+      <c r="C11" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="21" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="18" customHeight="1">
-      <c r="B12" s="19">
+      <c r="B12" s="18">
         <v>5</v>
       </c>
-      <c r="C12" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="25" t="s">
+      <c r="C12" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="22"/>
+      <c r="E12" s="23" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="18" customHeight="1">
-      <c r="B13" s="18">
+      <c r="B13" s="17">
         <v>60</v>
       </c>
-      <c r="C13" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="23" t="s">
+      <c r="C13" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="18" customHeight="1">
-      <c r="B14" s="19">
+      <c r="B14" s="18">
         <v>93.09</v>
       </c>
-      <c r="C14" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="25" t="s">
+      <c r="C14" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="22"/>
+      <c r="E14" s="23" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="18" customHeight="1">
-      <c r="B15" s="18">
+      <c r="B15" s="17">
         <v>181</v>
       </c>
-      <c r="C15" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="22"/>
-      <c r="E15" s="23" t="s">
+      <c r="C15" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1">
-      <c r="B16" s="19">
+      <c r="B16" s="18">
         <v>8</v>
       </c>
-      <c r="C16" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="25" t="s">
+      <c r="C16" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="22"/>
+      <c r="E16" s="23" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="18" customHeight="1">
-      <c r="B17" s="18">
-        <v>0</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="22"/>
-      <c r="E17" s="23" t="s">
+      <c r="B17" s="17">
+        <v>0</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="20"/>
+      <c r="E17" s="21" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="18" customHeight="1">
-      <c r="B18" s="26">
+      <c r="B18" s="24">
         <v>2</v>
       </c>
-      <c r="C18" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="25" t="s">
+      <c r="C18" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="22"/>
+      <c r="E18" s="23" t="s">
         <v>57</v>
       </c>
       <c r="G18" s="13"/>
     </row>
     <row r="19" spans="1:7" ht="18" customHeight="1">
-      <c r="B19" s="18">
-        <v>0</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="22"/>
-      <c r="E19" s="23" t="s">
+      <c r="B19" s="17">
+        <v>0</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="20"/>
+      <c r="E19" s="21" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="18" customHeight="1">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="19">
+      <c r="B20" s="18">
         <v>23.27</v>
       </c>
-      <c r="C20" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="25" t="s">
+      <c r="C20" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="22"/>
+      <c r="E20" s="23" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="18" customHeight="1">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="B21" s="18">
+      <c r="B21" s="17">
         <v>59</v>
       </c>
-      <c r="C21" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="22"/>
-      <c r="E21" s="23" t="s">
+      <c r="C21" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="20"/>
+      <c r="E21" s="21" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="18" customHeight="1">
-      <c r="A22" s="27"/>
-      <c r="B22" s="19">
+      <c r="A22" s="25"/>
+      <c r="B22" s="18">
         <v>50</v>
       </c>
-      <c r="C22" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="24"/>
-      <c r="E22" s="25" t="s">
+      <c r="C22" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="22"/>
+      <c r="E22" s="23" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="18" customHeight="1">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="18">
+      <c r="B23" s="17">
         <v>50</v>
       </c>
-      <c r="C23" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="22"/>
-      <c r="E23" s="23" t="s">
+      <c r="C23" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="20"/>
+      <c r="E23" s="21" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="18" customHeight="1">
-      <c r="A24" s="27"/>
-      <c r="B24" s="19">
-        <v>0</v>
-      </c>
-      <c r="C24" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" s="24"/>
-      <c r="E24" s="25" t="s">
+      <c r="A24" s="25"/>
+      <c r="B24" s="18">
+        <v>0</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="22"/>
+      <c r="E24" s="23" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="18" customHeight="1">
-      <c r="A25" s="27"/>
-      <c r="B25" s="18">
-        <v>0</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="22"/>
-      <c r="E25" s="23" t="s">
+      <c r="A25" s="25"/>
+      <c r="B25" s="17">
+        <v>0</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="20"/>
+      <c r="E25" s="21" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="18" customHeight="1">
-      <c r="A26" s="27"/>
-      <c r="B26" s="19">
-        <v>0</v>
-      </c>
-      <c r="C26" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" s="24"/>
-      <c r="E26" s="25" t="s">
+      <c r="A26" s="25"/>
+      <c r="B26" s="18">
+        <v>0</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="22"/>
+      <c r="E26" s="23" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="18" customHeight="1">
-      <c r="A27" s="27"/>
-      <c r="B27" s="18">
+      <c r="A27" s="25"/>
+      <c r="B27" s="17">
         <v>69.819999999999993</v>
       </c>
-      <c r="C27" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="D27" s="22"/>
-      <c r="E27" s="23" t="s">
+      <c r="C27" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="20"/>
+      <c r="E27" s="21" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="18" customHeight="1">
-      <c r="A28" s="27"/>
-      <c r="B28" s="19">
+      <c r="A28" s="25"/>
+      <c r="B28" s="18">
         <v>88</v>
       </c>
-      <c r="C28" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" s="24"/>
-      <c r="E28" s="25" t="s">
+      <c r="C28" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="22"/>
+      <c r="E28" s="23" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="18" customHeight="1">
-      <c r="B29" s="18">
+      <c r="B29" s="17">
         <v>50</v>
       </c>
-      <c r="C29" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="D29" s="22"/>
-      <c r="E29" s="23" t="s">
+      <c r="C29" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" s="20"/>
+      <c r="E29" s="21" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="18" customHeight="1">
-      <c r="B30" s="19">
+      <c r="B30" s="18">
         <v>50</v>
       </c>
-      <c r="C30" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="D30" s="24"/>
-      <c r="E30" s="25" t="s">
+      <c r="C30" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="22"/>
+      <c r="E30" s="23" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="18" customHeight="1">
-      <c r="B31" s="18">
-        <v>0</v>
-      </c>
-      <c r="C31" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="D31" s="22"/>
-      <c r="E31" s="23" t="s">
+      <c r="B31" s="17">
+        <v>0</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="20"/>
+      <c r="E31" s="21" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="18" customHeight="1">
-      <c r="B32" s="19">
-        <v>0</v>
-      </c>
-      <c r="C32" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="D32" s="24"/>
-      <c r="E32" s="25" t="s">
+      <c r="B32" s="18">
+        <v>0</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="22"/>
+      <c r="E32" s="23" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="33" spans="2:5" ht="18" customHeight="1">
-      <c r="B33" s="18">
-        <v>0</v>
-      </c>
-      <c r="C33" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="D33" s="22"/>
-      <c r="E33" s="23" t="s">
+      <c r="B33" s="17">
+        <v>0</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="20"/>
+      <c r="E33" s="21" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2156,7 +2156,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="74.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2164,7 +2164,7 @@
       <c r="A1" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>47</v>
       </c>
       <c r="C1" t="s">
@@ -2175,10 +2175,10 @@
       <c r="A2">
         <v>16</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="17" t="s">
+      <c r="B2" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2186,10 +2186,10 @@
       <c r="A3">
         <v>5</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="17" t="s">
+      <c r="B3" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2197,10 +2197,10 @@
       <c r="A4">
         <v>60</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="17" t="s">
+      <c r="B4" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2208,10 +2208,10 @@
       <c r="A5">
         <v>93.09</v>
       </c>
-      <c r="B5" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="17" t="s">
+      <c r="B5" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2219,10 +2219,10 @@
       <c r="A6">
         <v>181</v>
       </c>
-      <c r="B6" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="17" t="s">
+      <c r="B6" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2230,10 +2230,10 @@
       <c r="A7">
         <v>8</v>
       </c>
-      <c r="B7" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="17" t="s">
+      <c r="B7" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2241,10 +2241,10 @@
       <c r="A8">
         <v>0</v>
       </c>
-      <c r="B8" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="17" t="s">
+      <c r="B8" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2252,10 +2252,10 @@
       <c r="A9">
         <v>2</v>
       </c>
-      <c r="B9" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="17" t="s">
+      <c r="B9" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2263,10 +2263,10 @@
       <c r="A10">
         <v>0</v>
       </c>
-      <c r="B10" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="17" t="s">
+      <c r="B10" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2274,10 +2274,10 @@
       <c r="A11">
         <v>23.27</v>
       </c>
-      <c r="B11" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="17" t="s">
+      <c r="B11" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2285,10 +2285,10 @@
       <c r="A12">
         <v>59</v>
       </c>
-      <c r="B12" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="17" t="s">
+      <c r="B12" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2296,10 +2296,10 @@
       <c r="A13">
         <v>50</v>
       </c>
-      <c r="B13" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="17" t="s">
+      <c r="B13" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2307,10 +2307,10 @@
       <c r="A14">
         <v>50</v>
       </c>
-      <c r="B14" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="17" t="s">
+      <c r="B14" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2318,10 +2318,10 @@
       <c r="A15">
         <v>0</v>
       </c>
-      <c r="B15" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="17" t="s">
+      <c r="B15" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2329,10 +2329,10 @@
       <c r="A16">
         <v>0</v>
       </c>
-      <c r="B16" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="17" t="s">
+      <c r="B16" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2340,10 +2340,10 @@
       <c r="A17">
         <v>0</v>
       </c>
-      <c r="B17" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="17" t="s">
+      <c r="B17" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2351,10 +2351,10 @@
       <c r="A18">
         <v>69.819999999999993</v>
       </c>
-      <c r="B18" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="17" t="s">
+      <c r="B18" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2362,10 +2362,10 @@
       <c r="A19">
         <v>88</v>
       </c>
-      <c r="B19" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="17" t="s">
+      <c r="B19" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2373,10 +2373,10 @@
       <c r="A20">
         <v>50</v>
       </c>
-      <c r="B20" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="17" t="s">
+      <c r="B20" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2384,10 +2384,10 @@
       <c r="A21">
         <v>50</v>
       </c>
-      <c r="B21" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="17" t="s">
+      <c r="B21" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2395,10 +2395,10 @@
       <c r="A22">
         <v>0</v>
       </c>
-      <c r="B22" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="17" t="s">
+      <c r="B22" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2406,10 +2406,10 @@
       <c r="A23">
         <v>0</v>
       </c>
-      <c r="B23" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="17" t="s">
+      <c r="B23" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2417,10 +2417,10 @@
       <c r="A24">
         <v>0</v>
       </c>
-      <c r="B24" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="17" t="s">
+      <c r="B24" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>